<commit_message>
Broken pipeline, needs fixin
</commit_message>
<xml_diff>
--- a/Kristoffer betas/information dates/dates data.xlsx
+++ b/Kristoffer betas/information dates/dates data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KVKUNKEL/Documents/ITU/Git/Kristoffer betas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KVKUNKEL/Documents/ITU/Git/Kristoffer betas/information dates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
     <sheet name="dates" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1680,11 +1680,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-2055062256"/>
-        <c:axId val="-2053663888"/>
+        <c:axId val="-854486592"/>
+        <c:axId val="-939467888"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-2055062256"/>
+        <c:axId val="-854486592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1727,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053663888"/>
+        <c:crossAx val="-939467888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="50"/>
@@ -1735,7 +1735,7 @@
         <c:majorUnit val="12.0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2053663888"/>
+        <c:axId val="-939467888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,7 +1786,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055062256"/>
+        <c:crossAx val="-854486592"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2714,8 +2714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F211" workbookViewId="0">
-      <selection activeCell="K242" sqref="K242"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>